<commit_message>
update postprocessing to accompany resubmission
</commit_message>
<xml_diff>
--- a/data/demographics.xlsx
+++ b/data/demographics.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\NMBL\MM-CP\Barefoot Ambulator Paper\repo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD25E0A8-DE77-404C-82D8-9DECD640A7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="22695" windowHeight="14595"/>
   </bookViews>
   <sheets>
     <sheet name="primary subjects" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'primary subjects'!$A$2:$AA$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'primary subjects'!$A$2:$AB$34</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="79">
   <si>
     <t>sex</t>
   </si>
@@ -580,11 +579,17 @@
   <si>
     <t>none</t>
   </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>no R trials</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -667,7 +672,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -691,6 +696,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1014,77 +1022,79 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
+      <selection pane="bottomRight" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="9.1328125" style="1"/>
-    <col min="6" max="6" width="7.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="20.3984375" style="1" customWidth="1"/>
+    <col min="8" max="9" width="20.42578125" style="1" customWidth="1"/>
     <col min="10" max="10" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.73046875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="33.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.1328125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19" style="1" customWidth="1"/>
-    <col min="17" max="17" width="32.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="32.3984375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="19.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.1328125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="19.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.1328125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="23.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.73046875" style="1" customWidth="1"/>
-    <col min="25" max="26" width="29.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="9.1328125" style="1"/>
+    <col min="11" max="11" width="22" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="33.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19" style="1" customWidth="1"/>
+    <col min="18" max="18" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="32.42578125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.140625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.140625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.7109375" style="1" customWidth="1"/>
+    <col min="26" max="27" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="16" t="s">
+    <row r="1" spans="1:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="15" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="14" t="s">
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="13" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:28" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
@@ -1115,59 +1125,62 @@
       <c r="J2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="L2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="M2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="N2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="O2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="P2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="Q2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="R2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="S2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="S2" s="12" t="s">
+      <c r="T2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="12" t="s">
+      <c r="U2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="V2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="12" t="s">
+      <c r="W2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="W2" s="12" t="s">
+      <c r="X2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="X2" s="12" t="s">
+      <c r="Y2" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="Y2" s="12" t="s">
+      <c r="Z2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="Z2" s="12" t="s">
+      <c r="AA2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AA2" s="10" t="s">
+      <c r="AB2" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -1198,9 +1211,10 @@
       <c r="J3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AA3" s="5"/>
+      <c r="K3" s="2"/>
+      <c r="AB3" s="5"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>38</v>
       </c>
@@ -1231,9 +1245,10 @@
       <c r="J4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AA4" s="5"/>
+      <c r="K4" s="2"/>
+      <c r="AB4" s="5"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
@@ -1264,9 +1279,10 @@
       <c r="J5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AA5" s="5"/>
+      <c r="K5" s="2"/>
+      <c r="AB5" s="5"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
@@ -1297,9 +1313,10 @@
       <c r="J6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AA6" s="5"/>
+      <c r="K6" s="2"/>
+      <c r="AB6" s="5"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
@@ -1330,9 +1347,10 @@
       <c r="J7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AA7" s="5"/>
+      <c r="K7" s="2"/>
+      <c r="AB7" s="5"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
@@ -1363,9 +1381,10 @@
       <c r="J8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AA8" s="5"/>
+      <c r="K8" s="2"/>
+      <c r="AB8" s="5"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>40</v>
       </c>
@@ -1396,7 +1415,7 @@
       <c r="J9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K9" s="3"/>
+      <c r="K9" s="4"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
@@ -1412,9 +1431,10 @@
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
-      <c r="AA9" s="6"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="6"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
@@ -1445,57 +1465,58 @@
       <c r="J10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="2"/>
+      <c r="L10" s="1">
         <v>971.22681</v>
       </c>
-      <c r="L10" s="1">
+      <c r="M10" s="1">
         <v>869.18470000000002</v>
       </c>
-      <c r="M10" s="1">
+      <c r="N10" s="1">
         <v>67.314340000000001</v>
       </c>
-      <c r="N10" s="1">
+      <c r="O10" s="1">
         <v>132.13757000000001</v>
       </c>
-      <c r="O10" s="1">
+      <c r="P10" s="1">
         <v>764.62063000000001</v>
       </c>
-      <c r="P10" s="1">
+      <c r="Q10" s="1">
         <v>754.34185000000002</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="R10" s="1">
         <v>182.5017</v>
       </c>
-      <c r="R10" s="1">
+      <c r="S10" s="1">
         <v>150.75900999999999</v>
       </c>
-      <c r="S10" s="1">
+      <c r="T10" s="1">
         <v>188.69056</v>
       </c>
-      <c r="T10" s="1">
+      <c r="U10" s="1">
         <v>192.88788</v>
       </c>
-      <c r="U10" s="1">
+      <c r="V10" s="1">
         <v>274.15007000000003</v>
       </c>
-      <c r="V10" s="1">
+      <c r="W10" s="1">
         <v>261.54874000000001</v>
       </c>
-      <c r="W10" s="1">
+      <c r="X10" s="1">
         <v>4.12765</v>
       </c>
-      <c r="X10" s="1">
+      <c r="Y10" s="1">
         <v>4.3728899999999999</v>
       </c>
-      <c r="Y10" s="1">
+      <c r="Z10" s="1">
         <v>989.44574</v>
       </c>
-      <c r="Z10" s="1">
+      <c r="AA10" s="1">
         <v>1018.0657</v>
       </c>
-      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
@@ -1526,59 +1547,62 @@
       <c r="J11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L11" s="1">
         <v>557.17125999999996</v>
       </c>
-      <c r="L11" s="1">
+      <c r="M11" s="1">
         <v>572.91818999999998</v>
       </c>
-      <c r="M11" s="1">
+      <c r="N11" s="1">
         <v>115.86512999999999</v>
       </c>
-      <c r="N11" s="1">
+      <c r="O11" s="1">
         <v>124.21796999999999</v>
       </c>
-      <c r="O11" s="1">
+      <c r="P11" s="1">
         <v>414.76819999999998</v>
       </c>
-      <c r="P11" s="1">
+      <c r="Q11" s="1">
         <v>406.34141</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="R11" s="1">
         <v>95.378349999999998</v>
       </c>
-      <c r="R11" s="1">
+      <c r="S11" s="1">
         <v>96.339309999999998</v>
       </c>
-      <c r="S11" s="1">
+      <c r="T11" s="1">
         <v>131.9916637</v>
       </c>
-      <c r="T11" s="1">
+      <c r="U11" s="1">
         <v>132.79545450000001</v>
       </c>
-      <c r="U11" s="1">
+      <c r="V11" s="1">
         <v>171.00134019999999</v>
       </c>
-      <c r="V11" s="1">
+      <c r="W11" s="1">
         <v>174.98923859999999</v>
       </c>
-      <c r="W11" s="1">
+      <c r="X11" s="1">
         <v>3.862108793</v>
       </c>
-      <c r="X11" s="1">
+      <c r="Y11" s="1">
         <v>3.8245420289999998</v>
       </c>
-      <c r="Y11" s="1">
+      <c r="Z11" s="1">
         <v>935.15936199999999</v>
       </c>
-      <c r="Z11" s="1">
+      <c r="AA11" s="1">
         <v>924.54187130000003</v>
       </c>
-      <c r="AA11" s="2">
+      <c r="AB11" s="2">
         <v>12433.33333333333</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
@@ -1609,59 +1633,60 @@
       <c r="J12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="2"/>
+      <c r="L12" s="1">
         <v>732.51441999999997</v>
       </c>
-      <c r="L12" s="1">
+      <c r="M12" s="1">
         <v>758.66273000000001</v>
       </c>
-      <c r="M12" s="1">
+      <c r="N12" s="1">
         <v>125.27966000000001</v>
       </c>
-      <c r="N12" s="1">
+      <c r="O12" s="1">
         <v>153.15132</v>
       </c>
-      <c r="O12" s="1">
+      <c r="P12" s="1">
         <v>443.44835</v>
       </c>
-      <c r="P12" s="1">
+      <c r="Q12" s="1">
         <v>617.38238999999999</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="R12" s="1">
         <v>115.06483</v>
       </c>
-      <c r="R12" s="1">
+      <c r="S12" s="1">
         <v>135.63702000000001</v>
       </c>
-      <c r="S12" s="1">
+      <c r="T12" s="1">
         <v>194.5243787</v>
       </c>
-      <c r="T12" s="1">
+      <c r="U12" s="1">
         <v>208.9909016</v>
       </c>
-      <c r="U12" s="1">
+      <c r="V12" s="1">
         <v>303.47790029999999</v>
       </c>
-      <c r="V12" s="1">
+      <c r="W12" s="1">
         <v>324.15078510000001</v>
       </c>
-      <c r="W12" s="1">
+      <c r="X12" s="1">
         <v>3.9298678009999999</v>
       </c>
-      <c r="X12" s="1">
+      <c r="Y12" s="1">
         <v>4.1187787550000001</v>
       </c>
-      <c r="Y12" s="1">
+      <c r="Z12" s="1">
         <v>979.18874410000001</v>
       </c>
-      <c r="Z12" s="1">
+      <c r="AA12" s="1">
         <v>972.29186110000001</v>
       </c>
-      <c r="AA12" s="2">
+      <c r="AB12" s="2">
         <v>9525</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>47</v>
       </c>
@@ -1692,59 +1717,60 @@
       <c r="J13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="2"/>
+      <c r="L13" s="1">
         <v>895.42854</v>
       </c>
-      <c r="L13" s="1">
+      <c r="M13" s="1">
         <v>829.95164999999997</v>
       </c>
-      <c r="M13" s="1">
+      <c r="N13" s="1">
         <v>84.869200000000006</v>
       </c>
-      <c r="N13" s="1">
+      <c r="O13" s="1">
         <v>77.907870000000003</v>
       </c>
-      <c r="O13" s="1">
+      <c r="P13" s="1">
         <v>640.79589999999996</v>
       </c>
-      <c r="P13" s="1">
+      <c r="Q13" s="1">
         <v>657.92372</v>
       </c>
-      <c r="Q13" s="1">
+      <c r="R13" s="1">
         <v>144.29281</v>
       </c>
-      <c r="R13" s="1">
+      <c r="S13" s="1">
         <v>145.75214</v>
       </c>
-      <c r="S13" s="1">
+      <c r="T13" s="1">
         <v>261.52596</v>
       </c>
-      <c r="T13" s="1">
+      <c r="U13" s="1">
         <v>250.5590133</v>
       </c>
-      <c r="U13" s="1">
+      <c r="V13" s="1">
         <v>344.22816</v>
       </c>
-      <c r="V13" s="1">
+      <c r="W13" s="1">
         <v>337.28944990000002</v>
       </c>
-      <c r="W13" s="1">
+      <c r="X13" s="1">
         <v>5.3716400000000002</v>
       </c>
-      <c r="X13" s="1">
+      <c r="Y13" s="1">
         <v>5.1106531390000001</v>
       </c>
-      <c r="Y13" s="1">
+      <c r="Z13" s="1">
         <v>1107.23119</v>
       </c>
-      <c r="Z13" s="1">
+      <c r="AA13" s="1">
         <v>1106.72433</v>
       </c>
-      <c r="AA13" s="2">
+      <c r="AB13" s="2">
         <v>15959.6</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>48</v>
       </c>
@@ -1775,59 +1801,60 @@
       <c r="J14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="2"/>
+      <c r="L14" s="1">
         <v>1017.56678</v>
       </c>
-      <c r="L14" s="1">
+      <c r="M14" s="1">
         <v>1117.4777200000001</v>
       </c>
-      <c r="M14" s="1">
+      <c r="N14" s="1">
         <v>75.108040000000003</v>
       </c>
-      <c r="N14" s="1">
+      <c r="O14" s="1">
         <v>115.90119</v>
       </c>
-      <c r="O14" s="1">
+      <c r="P14" s="1">
         <v>789.42300999999998</v>
       </c>
-      <c r="P14" s="1">
+      <c r="Q14" s="1">
         <v>847.80092999999999</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="R14" s="1">
         <v>157.84951000000001</v>
       </c>
-      <c r="R14" s="1">
+      <c r="S14" s="1">
         <v>149.96414999999999</v>
       </c>
-      <c r="S14" s="1">
+      <c r="T14" s="1">
         <v>192.43742093887599</v>
       </c>
-      <c r="T14" s="1">
+      <c r="U14" s="1">
         <v>208.19268965559789</v>
       </c>
-      <c r="U14" s="1">
+      <c r="V14" s="1">
         <v>247.41880914397399</v>
       </c>
-      <c r="V14" s="1">
+      <c r="W14" s="1">
         <v>266.29384000129551</v>
       </c>
-      <c r="W14" s="1">
+      <c r="X14" s="1">
         <v>4.6837504792756146</v>
       </c>
-      <c r="X14" s="1">
+      <c r="Y14" s="1">
         <v>4.8730509187895317</v>
       </c>
-      <c r="Y14" s="1">
+      <c r="Z14" s="1">
         <v>1036.391858910358</v>
       </c>
-      <c r="Z14" s="1">
+      <c r="AA14" s="1">
         <v>1006.167728861249</v>
       </c>
-      <c r="AA14" s="2">
+      <c r="AB14" s="2">
         <v>6062.666666666667</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
@@ -1858,59 +1885,60 @@
       <c r="J15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="2"/>
+      <c r="L15" s="1">
         <v>543.59777999999994</v>
       </c>
-      <c r="L15" s="1">
+      <c r="M15" s="1">
         <v>559.87158999999997</v>
       </c>
-      <c r="M15" s="1">
+      <c r="N15" s="1">
         <v>145.15558999999999</v>
       </c>
-      <c r="N15" s="1">
+      <c r="O15" s="1">
         <v>141.20428000000001</v>
       </c>
-      <c r="O15" s="1">
+      <c r="P15" s="1">
         <v>379.14373999999998</v>
       </c>
-      <c r="P15" s="1">
+      <c r="Q15" s="1">
         <v>386.36266999999998</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="R15" s="1">
         <v>156.09083999999999</v>
       </c>
-      <c r="R15" s="1">
+      <c r="S15" s="1">
         <v>147.8646</v>
       </c>
-      <c r="S15" s="1">
+      <c r="T15" s="1">
         <v>156.7227244</v>
       </c>
-      <c r="T15" s="1">
+      <c r="U15" s="1">
         <v>157.0976781</v>
       </c>
-      <c r="U15" s="1">
+      <c r="V15" s="1">
         <v>194.72618209999999</v>
       </c>
-      <c r="V15" s="1">
+      <c r="W15" s="1">
         <v>199.49989790000001</v>
       </c>
-      <c r="W15" s="1">
+      <c r="X15" s="1">
         <v>4.395166101</v>
       </c>
-      <c r="X15" s="1">
+      <c r="Y15" s="1">
         <v>4.2790856049999997</v>
       </c>
-      <c r="Y15" s="1">
+      <c r="Z15" s="1">
         <v>1032.8462420000001</v>
       </c>
-      <c r="Z15" s="1">
+      <c r="AA15" s="1">
         <v>1028.397297</v>
       </c>
-      <c r="AA15" s="2">
+      <c r="AB15" s="2">
         <v>7512</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>50</v>
       </c>
@@ -1941,59 +1969,60 @@
       <c r="J16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="2"/>
+      <c r="L16" s="1">
         <v>888.20477000000005</v>
       </c>
-      <c r="L16" s="1">
+      <c r="M16" s="1">
         <v>922.38914</v>
       </c>
-      <c r="M16" s="1">
+      <c r="N16" s="1">
         <v>71.402720000000002</v>
       </c>
-      <c r="N16" s="1">
+      <c r="O16" s="1">
         <v>57.495759999999997</v>
       </c>
-      <c r="O16" s="1">
+      <c r="P16" s="1">
         <v>591.71541000000002</v>
       </c>
-      <c r="P16" s="1">
+      <c r="Q16" s="1">
         <v>628.66642999999999</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="R16" s="1">
         <v>142.8648</v>
       </c>
-      <c r="R16" s="1">
+      <c r="S16" s="1">
         <v>139.34009</v>
       </c>
-      <c r="S16" s="1">
+      <c r="T16" s="1">
         <v>190.13226</v>
       </c>
-      <c r="T16" s="1">
+      <c r="U16" s="1">
         <v>191.75372999999999</v>
       </c>
-      <c r="U16" s="1">
+      <c r="V16" s="1">
         <v>262.40213</v>
       </c>
-      <c r="V16" s="1">
+      <c r="W16" s="1">
         <v>269.39031</v>
       </c>
-      <c r="W16" s="1">
+      <c r="X16" s="1">
         <v>4.3298199999999998</v>
       </c>
-      <c r="X16" s="1">
+      <c r="Y16" s="1">
         <v>4.3219799999999999</v>
       </c>
-      <c r="Y16" s="1">
+      <c r="Z16" s="1">
         <v>1027.65796</v>
       </c>
-      <c r="Z16" s="1">
+      <c r="AA16" s="1">
         <v>997.96393</v>
       </c>
-      <c r="AA16" s="2">
+      <c r="AB16" s="2">
         <v>12579.428571428571</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>51</v>
       </c>
@@ -2024,57 +2053,60 @@
       <c r="J17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L17" s="1">
         <v>567.35514999999998</v>
       </c>
-      <c r="L17" s="1">
+      <c r="M17" s="1">
         <v>566.75945999999999</v>
       </c>
-      <c r="M17" s="1">
+      <c r="N17" s="1">
         <v>152.24665999999999</v>
       </c>
-      <c r="N17" s="1">
+      <c r="O17" s="1">
         <v>155.45326</v>
       </c>
-      <c r="O17" s="1">
+      <c r="P17" s="1">
         <v>379.19549999999998</v>
       </c>
-      <c r="P17" s="1">
+      <c r="Q17" s="1">
         <v>461.61520999999999</v>
       </c>
-      <c r="Q17" s="1">
+      <c r="R17" s="1">
         <v>116.1187</v>
       </c>
-      <c r="R17" s="1">
+      <c r="S17" s="1">
         <v>124.30761</v>
       </c>
-      <c r="S17" s="1">
+      <c r="T17" s="1">
         <v>136.79400999999999</v>
       </c>
-      <c r="T17" s="1">
+      <c r="U17" s="1">
         <v>150.59387000000001</v>
       </c>
-      <c r="U17" s="1">
+      <c r="V17" s="1">
         <v>186.53021000000001</v>
       </c>
-      <c r="V17" s="1">
+      <c r="W17" s="1">
         <v>201.79184000000001</v>
       </c>
-      <c r="W17" s="1">
+      <c r="X17" s="1">
         <v>3.74776</v>
       </c>
-      <c r="X17" s="1">
+      <c r="Y17" s="1">
         <v>3.9779599999999999</v>
       </c>
-      <c r="Y17" s="1">
+      <c r="Z17" s="1">
         <v>962.55337999999995</v>
       </c>
-      <c r="Z17" s="1">
+      <c r="AA17" s="1">
         <v>943.60472000000004</v>
       </c>
-      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>52</v>
       </c>
@@ -2105,59 +2137,60 @@
       <c r="J18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18" s="2"/>
+      <c r="L18" s="1">
         <v>741.47811999999999</v>
       </c>
-      <c r="L18" s="1">
+      <c r="M18" s="1">
         <v>698.01855</v>
       </c>
-      <c r="M18" s="1">
+      <c r="N18" s="1">
         <v>130.31726</v>
       </c>
-      <c r="N18" s="1">
+      <c r="O18" s="1">
         <v>118.60429000000001</v>
       </c>
-      <c r="O18" s="1">
+      <c r="P18" s="1">
         <v>502.99592999999999</v>
       </c>
-      <c r="P18" s="1">
+      <c r="Q18" s="1">
         <v>489.85097000000002</v>
       </c>
-      <c r="Q18" s="1">
+      <c r="R18" s="1">
         <v>140.56599</v>
       </c>
-      <c r="R18" s="1">
+      <c r="S18" s="1">
         <v>136.26911000000001</v>
       </c>
-      <c r="S18" s="1">
+      <c r="T18" s="1">
         <v>213.98281</v>
       </c>
-      <c r="T18" s="1">
+      <c r="U18" s="1">
         <v>204.86033</v>
       </c>
-      <c r="U18" s="1">
+      <c r="V18" s="1">
         <v>273.68074999999999</v>
       </c>
-      <c r="V18" s="1">
+      <c r="W18" s="1">
         <v>265.55032</v>
       </c>
-      <c r="W18" s="1">
+      <c r="X18" s="1">
         <v>4.9659300000000002</v>
       </c>
-      <c r="X18" s="1">
+      <c r="Y18" s="1">
         <v>4.7678799999999999</v>
       </c>
-      <c r="Y18" s="1">
+      <c r="Z18" s="1">
         <v>956.82394999999997</v>
       </c>
-      <c r="Z18" s="1">
+      <c r="AA18" s="1">
         <v>961.69502999999997</v>
       </c>
-      <c r="AA18" s="2">
+      <c r="AB18" s="2">
         <v>5571.7142857142853</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>53</v>
       </c>
@@ -2188,59 +2221,60 @@
       <c r="J19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K19" s="1">
+      <c r="K19" s="2"/>
+      <c r="L19" s="1">
         <v>1031.3882799999999</v>
       </c>
-      <c r="L19" s="1">
+      <c r="M19" s="1">
         <v>1137.83349</v>
       </c>
-      <c r="M19" s="1">
+      <c r="N19" s="1">
         <v>91.73039</v>
       </c>
-      <c r="N19" s="1">
+      <c r="O19" s="1">
         <v>91.051760000000002</v>
       </c>
-      <c r="O19" s="1">
+      <c r="P19" s="1">
         <v>742.19231000000002</v>
       </c>
-      <c r="P19" s="1">
+      <c r="Q19" s="1">
         <v>749.62183000000005</v>
       </c>
-      <c r="Q19" s="1">
+      <c r="R19" s="1">
         <v>115.5116</v>
       </c>
-      <c r="R19" s="1">
+      <c r="S19" s="1">
         <v>127.33214</v>
       </c>
-      <c r="S19" s="1">
+      <c r="T19" s="1">
         <v>265.0855914</v>
       </c>
-      <c r="T19" s="1">
+      <c r="U19" s="1">
         <v>267.38682460000001</v>
       </c>
-      <c r="U19" s="1">
+      <c r="V19" s="1">
         <v>325.6342818</v>
       </c>
-      <c r="V19" s="1">
+      <c r="W19" s="1">
         <v>326.57241820000002</v>
       </c>
-      <c r="W19" s="1">
+      <c r="X19" s="1">
         <v>5.8772525599999996</v>
       </c>
-      <c r="X19" s="1">
+      <c r="Y19" s="1">
         <v>5.9387060250000001</v>
       </c>
-      <c r="Y19" s="1">
+      <c r="Z19" s="1">
         <v>1087.524228</v>
       </c>
-      <c r="Z19" s="1">
+      <c r="AA19" s="1">
         <v>1086.6669320000001</v>
       </c>
-      <c r="AA19" s="2">
+      <c r="AB19" s="2">
         <v>8208</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
@@ -2271,59 +2305,60 @@
       <c r="J20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K20" s="2"/>
+      <c r="L20" s="1">
         <v>892.33639000000005</v>
       </c>
-      <c r="L20" s="1">
+      <c r="M20" s="1">
         <v>903.09424000000001</v>
       </c>
-      <c r="M20" s="1">
+      <c r="N20" s="1">
         <v>112.00346999999999</v>
       </c>
-      <c r="N20" s="1">
+      <c r="O20" s="1">
         <v>103.52061</v>
       </c>
-      <c r="O20" s="1">
+      <c r="P20" s="1">
         <v>664.14131999999995</v>
       </c>
-      <c r="P20" s="1">
+      <c r="Q20" s="1">
         <v>691.12195999999994</v>
       </c>
-      <c r="Q20" s="1">
+      <c r="R20" s="1">
         <v>131.97758999999999</v>
       </c>
-      <c r="R20" s="1">
+      <c r="S20" s="1">
         <v>113.82752000000001</v>
       </c>
-      <c r="S20" s="1">
+      <c r="T20" s="1">
         <v>217.3621886</v>
       </c>
-      <c r="T20" s="1">
+      <c r="U20" s="1">
         <v>230.59550609999999</v>
       </c>
-      <c r="U20" s="1">
+      <c r="V20" s="1">
         <v>266.19015180000002</v>
       </c>
-      <c r="V20" s="1">
+      <c r="W20" s="1">
         <v>283.47891929999997</v>
       </c>
-      <c r="W20" s="1">
+      <c r="X20" s="1">
         <v>5.2651563340000003</v>
       </c>
-      <c r="X20" s="1">
+      <c r="Y20" s="1">
         <v>5.3812127419999998</v>
       </c>
-      <c r="Y20" s="1">
+      <c r="Z20" s="1">
         <v>1104.5243969999999</v>
       </c>
-      <c r="Z20" s="1">
+      <c r="AA20" s="1">
         <v>1107.550266</v>
       </c>
-      <c r="AA20" s="2">
+      <c r="AB20" s="2">
         <v>9587</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
@@ -2354,59 +2389,60 @@
       <c r="J21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K21" s="2"/>
+      <c r="L21" s="1">
         <v>1044.8938599999999</v>
       </c>
-      <c r="L21" s="1">
+      <c r="M21" s="1">
         <v>1014.68499</v>
       </c>
-      <c r="M21" s="1">
+      <c r="N21" s="1">
         <v>106.02646</v>
       </c>
-      <c r="N21" s="1">
+      <c r="O21" s="1">
         <v>112.70014999999999</v>
       </c>
-      <c r="O21" s="1">
+      <c r="P21" s="1">
         <v>774.32105000000001</v>
       </c>
-      <c r="P21" s="1">
+      <c r="Q21" s="1">
         <v>718.04052999999999</v>
       </c>
-      <c r="Q21" s="1">
+      <c r="R21" s="1">
         <v>152.61275000000001</v>
       </c>
-      <c r="R21" s="1">
+      <c r="S21" s="1">
         <v>161.60317000000001</v>
       </c>
-      <c r="S21" s="1">
+      <c r="T21" s="1">
         <v>211.81084680000001</v>
       </c>
-      <c r="T21" s="1">
+      <c r="U21" s="1">
         <v>206.1753368</v>
       </c>
-      <c r="U21" s="1">
+      <c r="V21" s="1">
         <v>280.03173670000001</v>
       </c>
-      <c r="V21" s="1">
+      <c r="W21" s="1">
         <v>271.34300339999999</v>
       </c>
-      <c r="W21" s="1">
+      <c r="X21" s="1">
         <v>4.7349204580000004</v>
       </c>
-      <c r="X21" s="1">
+      <c r="Y21" s="1">
         <v>4.713167887</v>
       </c>
-      <c r="Y21" s="1">
+      <c r="Z21" s="1">
         <v>1006.4030299999999</v>
       </c>
-      <c r="Z21" s="1">
+      <c r="AA21" s="1">
         <v>990.82983960000001</v>
       </c>
-      <c r="AA21" s="2">
+      <c r="AB21" s="2">
         <v>11074.222222222221</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>56</v>
       </c>
@@ -2437,59 +2473,62 @@
       <c r="J22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K22" s="1">
+      <c r="K22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L22" s="1">
         <v>445.77618999999999</v>
       </c>
-      <c r="L22" s="1">
+      <c r="M22" s="1">
         <v>457.66431</v>
       </c>
-      <c r="M22" s="1">
+      <c r="N22" s="1">
         <v>166.42495</v>
       </c>
-      <c r="N22" s="1">
+      <c r="O22" s="1">
         <v>170.34352999999999</v>
       </c>
-      <c r="O22" s="1">
+      <c r="P22" s="1">
         <v>302.75731999999999</v>
       </c>
-      <c r="P22" s="1">
+      <c r="Q22" s="1">
         <v>303.46298999999999</v>
       </c>
-      <c r="Q22" s="1">
+      <c r="R22" s="1">
         <v>135.25273999999999</v>
       </c>
-      <c r="R22" s="1">
+      <c r="S22" s="1">
         <v>146.92762999999999</v>
       </c>
-      <c r="S22" s="1">
+      <c r="T22" s="1">
         <v>136.17250999999999</v>
       </c>
-      <c r="T22" s="1">
+      <c r="U22" s="1">
         <v>130.74997999999999</v>
       </c>
-      <c r="U22" s="1">
+      <c r="V22" s="1">
         <v>176.91098</v>
       </c>
-      <c r="V22" s="1">
+      <c r="W22" s="1">
         <v>170.79979</v>
       </c>
-      <c r="W22" s="1">
+      <c r="X22" s="1">
         <v>3.9037999999999999</v>
       </c>
-      <c r="X22" s="1">
+      <c r="Y22" s="1">
         <v>3.7982499999999999</v>
       </c>
-      <c r="Y22" s="1">
+      <c r="Z22" s="1">
         <v>927.81208000000004</v>
       </c>
-      <c r="Z22" s="1">
+      <c r="AA22" s="1">
         <v>918.23526000000004</v>
       </c>
-      <c r="AA22" s="2">
+      <c r="AB22" s="2">
         <v>11716</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>57</v>
       </c>
@@ -2520,59 +2559,60 @@
       <c r="J23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K23" s="1">
+      <c r="K23" s="2"/>
+      <c r="L23" s="1">
         <v>1018.50119</v>
       </c>
-      <c r="L23" s="1">
+      <c r="M23" s="1">
         <v>1065.8293699999999</v>
       </c>
-      <c r="M23" s="1">
+      <c r="N23" s="1">
         <v>84.453829999999996</v>
       </c>
-      <c r="N23" s="1">
+      <c r="O23" s="1">
         <v>92.244299999999996</v>
       </c>
-      <c r="O23" s="1">
+      <c r="P23" s="1">
         <v>712.05687</v>
       </c>
-      <c r="P23" s="1">
+      <c r="Q23" s="1">
         <v>682.56370000000004</v>
       </c>
-      <c r="Q23" s="1">
+      <c r="R23" s="1">
         <v>146.02603999999999</v>
       </c>
-      <c r="R23" s="1">
+      <c r="S23" s="1">
         <v>138.14474000000001</v>
       </c>
-      <c r="S23" s="1">
+      <c r="T23" s="1">
         <v>248.80397490303491</v>
       </c>
-      <c r="T23" s="1">
+      <c r="U23" s="1">
         <v>271.80199863728308</v>
       </c>
-      <c r="U23" s="1">
+      <c r="V23" s="1">
         <v>340.36085227624659</v>
       </c>
-      <c r="V23" s="1">
+      <c r="W23" s="1">
         <v>361.82506502136812</v>
       </c>
-      <c r="W23" s="1">
+      <c r="X23" s="1">
         <v>4.9835347512336856</v>
       </c>
-      <c r="X23" s="1">
+      <c r="Y23" s="1">
         <v>5.3842879555983778</v>
       </c>
-      <c r="Y23" s="1">
+      <c r="Z23" s="1">
         <v>1033.9281328844611</v>
       </c>
-      <c r="Z23" s="1">
+      <c r="AA23" s="1">
         <v>1024.738412225076</v>
       </c>
-      <c r="AA23" s="2">
+      <c r="AB23" s="2">
         <v>4452</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>58</v>
       </c>
@@ -2603,59 +2643,60 @@
       <c r="J24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K24" s="2"/>
+      <c r="L24" s="1">
         <v>1423.50982</v>
       </c>
-      <c r="L24" s="1">
+      <c r="M24" s="1">
         <v>1459.74612</v>
       </c>
-      <c r="M24" s="1">
+      <c r="N24" s="1">
         <v>202.32382000000001</v>
       </c>
-      <c r="N24" s="1">
+      <c r="O24" s="1">
         <v>198.24880999999999</v>
       </c>
-      <c r="O24" s="1">
+      <c r="P24" s="1">
         <v>920.08424000000002</v>
       </c>
-      <c r="P24" s="1">
+      <c r="Q24" s="1">
         <v>902.50638000000004</v>
       </c>
-      <c r="Q24" s="1">
+      <c r="R24" s="1">
         <v>265.70513999999997</v>
       </c>
-      <c r="R24" s="1">
+      <c r="S24" s="1">
         <v>256.77848999999998</v>
       </c>
-      <c r="S24" s="1">
+      <c r="T24" s="1">
         <v>435.56657000000001</v>
       </c>
-      <c r="T24" s="1">
+      <c r="U24" s="1">
         <v>429.86572999999999</v>
       </c>
-      <c r="U24" s="1">
+      <c r="V24" s="1">
         <v>530.50761999999997</v>
       </c>
-      <c r="V24" s="1">
+      <c r="W24" s="1">
         <v>534.06164999999999</v>
       </c>
-      <c r="W24" s="1">
+      <c r="X24" s="1">
         <v>7.7128899999999998</v>
       </c>
-      <c r="X24" s="1">
+      <c r="Y24" s="1">
         <v>7.4000399999999997</v>
       </c>
-      <c r="Y24" s="1">
+      <c r="Z24" s="1">
         <v>1100.8772100000001</v>
       </c>
-      <c r="Z24" s="1">
+      <c r="AA24" s="1">
         <v>1105.8501799999999</v>
       </c>
-      <c r="AA24" s="2">
+      <c r="AB24" s="2">
         <v>8281.3333333333339</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>59</v>
       </c>
@@ -2686,59 +2727,60 @@
       <c r="J25" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K25" s="3">
+      <c r="K25" s="4"/>
+      <c r="L25" s="3">
         <v>1524.69163</v>
       </c>
-      <c r="L25" s="3">
+      <c r="M25" s="3">
         <v>1517.6020799999999</v>
       </c>
-      <c r="M25" s="3">
+      <c r="N25" s="3">
         <v>94.185199999999995</v>
       </c>
-      <c r="N25" s="3">
+      <c r="O25" s="3">
         <v>92.83211</v>
       </c>
-      <c r="O25" s="3">
+      <c r="P25" s="3">
         <v>937.01156000000003</v>
       </c>
-      <c r="P25" s="3">
+      <c r="Q25" s="3">
         <v>963.18377999999996</v>
       </c>
-      <c r="Q25" s="3">
+      <c r="R25" s="3">
         <v>152.36612</v>
       </c>
-      <c r="R25" s="3">
+      <c r="S25" s="3">
         <v>137.2621</v>
       </c>
-      <c r="S25" s="3">
+      <c r="T25" s="3">
         <v>444.63722239999998</v>
       </c>
-      <c r="T25" s="3">
+      <c r="U25" s="3">
         <v>436.11179329999999</v>
       </c>
-      <c r="U25" s="3">
+      <c r="V25" s="3">
         <v>545.64297509999994</v>
       </c>
-      <c r="V25" s="3">
+      <c r="W25" s="3">
         <v>533.47555550000004</v>
       </c>
-      <c r="W25" s="3">
+      <c r="X25" s="3">
         <v>7.5792933629999997</v>
       </c>
-      <c r="X25" s="3">
+      <c r="Y25" s="3">
         <v>7.5319988220000003</v>
       </c>
-      <c r="Y25" s="3">
+      <c r="Z25" s="3">
         <v>1101.7386630000001</v>
       </c>
-      <c r="Z25" s="3">
+      <c r="AA25" s="3">
         <v>1092.0736879999999</v>
       </c>
-      <c r="AA25" s="4">
+      <c r="AB25" s="4">
         <v>12225</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>72</v>
       </c>
@@ -2765,57 +2807,58 @@
       <c r="J26" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K26" s="1">
+      <c r="K26" s="2"/>
+      <c r="L26" s="1">
         <v>1093.8387299999999</v>
       </c>
-      <c r="L26" s="1">
+      <c r="M26" s="1">
         <v>1087.16472</v>
       </c>
-      <c r="M26" s="1">
+      <c r="N26" s="1">
         <v>246.55992000000001</v>
       </c>
-      <c r="N26" s="1">
+      <c r="O26" s="1">
         <v>226.14744999999999</v>
       </c>
-      <c r="O26" s="1">
+      <c r="P26" s="1">
         <v>709.3596</v>
       </c>
-      <c r="P26" s="1">
+      <c r="Q26" s="1">
         <v>729.53872000000001</v>
       </c>
-      <c r="Q26" s="1">
+      <c r="R26" s="1">
         <v>250.90967000000001</v>
       </c>
-      <c r="R26" s="1">
+      <c r="S26" s="1">
         <v>246.55885000000001</v>
       </c>
-      <c r="S26" s="1">
+      <c r="T26" s="1">
         <v>360.79689000000002</v>
       </c>
-      <c r="T26" s="1">
+      <c r="U26" s="1">
         <v>345.43182000000002</v>
       </c>
-      <c r="U26" s="1">
+      <c r="V26" s="1">
         <v>423.36275999999998</v>
       </c>
-      <c r="V26" s="1">
+      <c r="W26" s="1">
         <v>417.36543999999998</v>
       </c>
-      <c r="W26" s="1">
+      <c r="X26" s="1">
         <v>7.0027400000000002</v>
       </c>
-      <c r="X26" s="1">
+      <c r="Y26" s="1">
         <v>6.8222500000000004</v>
       </c>
-      <c r="Y26" s="1">
+      <c r="Z26" s="1">
         <v>1105.4894099999999</v>
       </c>
-      <c r="Z26" s="1">
+      <c r="AA26" s="1">
         <v>1096.5398299999999</v>
       </c>
-      <c r="AA26" s="2"/>
+      <c r="AB26" s="2"/>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>69</v>
       </c>
@@ -2842,57 +2885,58 @@
       <c r="J27" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K27" s="1">
+      <c r="K27" s="2"/>
+      <c r="L27" s="1">
         <v>979.80627000000004</v>
       </c>
-      <c r="L27" s="1">
+      <c r="M27" s="1">
         <v>1036.1970899999999</v>
       </c>
-      <c r="M27" s="1">
+      <c r="N27" s="1">
         <v>153.14598000000001</v>
       </c>
-      <c r="N27" s="1">
+      <c r="O27" s="1">
         <v>145.51114999999999</v>
       </c>
-      <c r="O27" s="1">
+      <c r="P27" s="1">
         <v>853.58961999999997</v>
       </c>
-      <c r="P27" s="1">
+      <c r="Q27" s="1">
         <v>889.49501999999995</v>
       </c>
-      <c r="Q27" s="1">
+      <c r="R27" s="1">
         <v>191.25721999999999</v>
       </c>
-      <c r="R27" s="1">
+      <c r="S27" s="1">
         <v>203.52283</v>
       </c>
-      <c r="S27" s="1">
+      <c r="T27" s="1">
         <v>303.39798780000001</v>
       </c>
-      <c r="T27" s="1">
+      <c r="U27" s="1">
         <v>299.6424308</v>
       </c>
-      <c r="U27" s="1">
+      <c r="V27" s="1">
         <v>390.6053182</v>
       </c>
-      <c r="V27" s="1">
+      <c r="W27" s="1">
         <v>393.01932770000002</v>
       </c>
-      <c r="W27" s="1">
+      <c r="X27" s="1">
         <v>5.930538179</v>
       </c>
-      <c r="X27" s="1">
+      <c r="Y27" s="1">
         <v>5.8858368490000004</v>
       </c>
-      <c r="Y27" s="1">
+      <c r="Z27" s="1">
         <v>1013.838078</v>
       </c>
-      <c r="Z27" s="1">
+      <c r="AA27" s="1">
         <v>1013.850279</v>
       </c>
-      <c r="AA27" s="2"/>
+      <c r="AB27" s="2"/>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>62</v>
       </c>
@@ -2919,57 +2963,58 @@
       <c r="J28" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K28" s="1">
+      <c r="K28" s="2"/>
+      <c r="L28" s="1">
         <v>683.35024999999996</v>
       </c>
-      <c r="L28" s="1">
+      <c r="M28" s="1">
         <v>652.77976000000001</v>
       </c>
-      <c r="M28" s="1">
+      <c r="N28" s="1">
         <v>199.08096</v>
       </c>
-      <c r="N28" s="1">
+      <c r="O28" s="1">
         <v>202.56598</v>
       </c>
-      <c r="O28" s="1">
+      <c r="P28" s="1">
         <v>437.98169000000001</v>
       </c>
-      <c r="P28" s="1">
+      <c r="Q28" s="1">
         <v>458.34372000000002</v>
       </c>
-      <c r="Q28" s="1">
+      <c r="R28" s="1">
         <v>119.56498000000001</v>
       </c>
-      <c r="R28" s="1">
+      <c r="S28" s="1">
         <v>136.06166999999999</v>
-      </c>
-      <c r="S28" s="1">
-        <v>171.04443810000001</v>
       </c>
       <c r="T28" s="1">
         <v>171.04443810000001</v>
       </c>
       <c r="U28" s="1">
-        <v>233.6392166</v>
+        <v>171.04443810000001</v>
       </c>
       <c r="V28" s="1">
         <v>233.6392166</v>
       </c>
       <c r="W28" s="1">
+        <v>233.6392166</v>
+      </c>
+      <c r="X28" s="1">
         <v>4.1380924889999999</v>
       </c>
-      <c r="X28" s="1">
+      <c r="Y28" s="1">
         <v>4.1380534229999997</v>
-      </c>
-      <c r="Y28" s="1">
-        <v>885.66641219999997</v>
       </c>
       <c r="Z28" s="1">
         <v>885.66641219999997</v>
       </c>
-      <c r="AA28" s="2"/>
+      <c r="AA28" s="1">
+        <v>885.66641219999997</v>
+      </c>
+      <c r="AB28" s="2"/>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>61</v>
       </c>
@@ -2996,57 +3041,58 @@
       <c r="J29" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K29" s="1">
+      <c r="K29" s="2"/>
+      <c r="L29" s="1">
         <v>881.17244000000005</v>
       </c>
-      <c r="L29" s="1">
+      <c r="M29" s="1">
         <v>913.79076999999995</v>
       </c>
-      <c r="M29" s="1">
+      <c r="N29" s="1">
         <v>141.69075000000001</v>
       </c>
-      <c r="N29" s="1">
+      <c r="O29" s="1">
         <v>145.53163000000001</v>
       </c>
-      <c r="O29" s="1">
+      <c r="P29" s="1">
         <v>806.85802000000001</v>
       </c>
-      <c r="P29" s="1">
+      <c r="Q29" s="1">
         <v>950.83022000000005</v>
       </c>
-      <c r="Q29" s="1">
+      <c r="R29" s="1">
         <v>137.22640999999999</v>
       </c>
-      <c r="R29" s="1">
+      <c r="S29" s="1">
         <v>149.10230000000001</v>
       </c>
-      <c r="S29" s="1">
+      <c r="T29" s="1">
         <v>228.47343720000001</v>
       </c>
-      <c r="T29" s="1">
+      <c r="U29" s="1">
         <v>238.59854659999999</v>
       </c>
-      <c r="U29" s="1">
+      <c r="V29" s="1">
         <v>282.96206050000001</v>
       </c>
-      <c r="V29" s="1">
+      <c r="W29" s="1">
         <v>292.95281679999999</v>
       </c>
-      <c r="W29" s="1">
+      <c r="X29" s="1">
         <v>5.4013238609999998</v>
       </c>
-      <c r="X29" s="1">
+      <c r="Y29" s="1">
         <v>5.5806706210000003</v>
       </c>
-      <c r="Y29" s="1">
+      <c r="Z29" s="1">
         <v>1019.943026</v>
       </c>
-      <c r="Z29" s="1">
+      <c r="AA29" s="1">
         <v>1010.976972</v>
       </c>
-      <c r="AA29" s="2"/>
+      <c r="AB29" s="2"/>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>67</v>
       </c>
@@ -3073,57 +3119,58 @@
       <c r="J30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K30" s="2"/>
+      <c r="L30" s="1">
         <v>526.92596000000003</v>
       </c>
-      <c r="L30" s="1">
+      <c r="M30" s="1">
         <v>533.53333999999995</v>
       </c>
-      <c r="M30" s="1">
+      <c r="N30" s="1">
         <v>169.33497</v>
       </c>
-      <c r="N30" s="1">
+      <c r="O30" s="1">
         <v>169.06312</v>
       </c>
-      <c r="O30" s="1">
+      <c r="P30" s="1">
         <v>387.39222999999998</v>
       </c>
-      <c r="P30" s="1">
+      <c r="Q30" s="1">
         <v>370.28917999999999</v>
       </c>
-      <c r="Q30" s="1">
+      <c r="R30" s="1">
         <v>130.48851999999999</v>
       </c>
-      <c r="R30" s="1">
+      <c r="S30" s="1">
         <v>125.77087</v>
       </c>
-      <c r="S30" s="1">
+      <c r="T30" s="1">
         <v>148.260076303869</v>
       </c>
-      <c r="T30" s="1">
+      <c r="U30" s="1">
         <v>144.36961976860081</v>
       </c>
-      <c r="U30" s="1">
+      <c r="V30" s="1">
         <v>183.5640202892944</v>
       </c>
-      <c r="V30" s="1">
+      <c r="W30" s="1">
         <v>178.92102407675699</v>
       </c>
-      <c r="W30" s="1">
+      <c r="X30" s="1">
         <v>4.2836305745092211</v>
       </c>
-      <c r="X30" s="1">
+      <c r="Y30" s="1">
         <v>4.2143742310469108</v>
       </c>
-      <c r="Y30" s="1">
+      <c r="Z30" s="1">
         <v>994.14464654578421</v>
       </c>
-      <c r="Z30" s="1">
+      <c r="AA30" s="1">
         <v>995.6130697293014</v>
       </c>
-      <c r="AA30" s="2"/>
+      <c r="AB30" s="2"/>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>68</v>
       </c>
@@ -3150,57 +3197,58 @@
       <c r="J31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K31" s="1">
+      <c r="K31" s="2"/>
+      <c r="L31" s="1">
         <v>785.20925999999997</v>
       </c>
-      <c r="L31" s="1">
+      <c r="M31" s="1">
         <v>818.34289999999999</v>
       </c>
-      <c r="M31" s="1">
+      <c r="N31" s="1">
         <v>120.958</v>
       </c>
-      <c r="N31" s="1">
+      <c r="O31" s="1">
         <v>110.69226999999999</v>
       </c>
-      <c r="O31" s="1">
+      <c r="P31" s="1">
         <v>578.75546999999995</v>
       </c>
-      <c r="P31" s="1">
+      <c r="Q31" s="1">
         <v>587.54278999999997</v>
       </c>
-      <c r="Q31" s="1">
+      <c r="R31" s="1">
         <v>125.97664</v>
       </c>
-      <c r="R31" s="1">
+      <c r="S31" s="1">
         <v>138.92929000000001</v>
       </c>
-      <c r="S31" s="1">
+      <c r="T31" s="1">
         <v>188.5061757228757</v>
       </c>
-      <c r="T31" s="1">
+      <c r="U31" s="1">
         <v>188.93015209999999</v>
       </c>
-      <c r="U31" s="1">
+      <c r="V31" s="1">
         <v>263.56519118998591</v>
       </c>
-      <c r="V31" s="1">
+      <c r="W31" s="1">
         <v>261.437095</v>
       </c>
-      <c r="W31" s="1">
+      <c r="X31" s="1">
         <v>4.2469356534420237</v>
       </c>
-      <c r="X31" s="1">
+      <c r="Y31" s="1">
         <v>4.3201197640000002</v>
       </c>
-      <c r="Y31" s="1">
+      <c r="Z31" s="1">
         <v>994.98870550550362</v>
       </c>
-      <c r="Z31" s="1">
+      <c r="AA31" s="1">
         <v>989.58130619999997</v>
       </c>
-      <c r="AA31" s="2"/>
+      <c r="AB31" s="2"/>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>66</v>
       </c>
@@ -3227,57 +3275,58 @@
       <c r="J32" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K32" s="1">
+      <c r="K32" s="2"/>
+      <c r="L32" s="1">
         <v>674.91783999999996</v>
       </c>
-      <c r="L32" s="1">
+      <c r="M32" s="1">
         <v>657.19036000000006</v>
       </c>
-      <c r="M32" s="1">
+      <c r="N32" s="1">
         <v>161.95015000000001</v>
       </c>
-      <c r="N32" s="1">
+      <c r="O32" s="1">
         <v>170.86046999999999</v>
       </c>
-      <c r="O32" s="1">
+      <c r="P32" s="1">
         <v>525.48843999999997</v>
       </c>
-      <c r="P32" s="1">
+      <c r="Q32" s="1">
         <v>524.37674000000004</v>
       </c>
-      <c r="Q32" s="1">
+      <c r="R32" s="1">
         <v>135.28971999999999</v>
       </c>
-      <c r="R32" s="1">
+      <c r="S32" s="1">
         <v>115.60209</v>
       </c>
-      <c r="S32" s="1">
+      <c r="T32" s="1">
         <v>212.34002823436691</v>
       </c>
-      <c r="T32" s="1">
+      <c r="U32" s="1">
         <v>206.29587915825269</v>
       </c>
-      <c r="U32" s="1">
+      <c r="V32" s="1">
         <v>268.59632973367451</v>
       </c>
-      <c r="V32" s="1">
+      <c r="W32" s="1">
         <v>257.14480987003299</v>
       </c>
-      <c r="W32" s="1">
+      <c r="X32" s="1">
         <v>5.0027844975746811</v>
       </c>
-      <c r="X32" s="1">
+      <c r="Y32" s="1">
         <v>5.0694248155336421</v>
       </c>
-      <c r="Y32" s="1">
+      <c r="Z32" s="1">
         <v>967.38141142984387</v>
       </c>
-      <c r="Z32" s="1">
+      <c r="AA32" s="1">
         <v>960.5710576595601</v>
       </c>
-      <c r="AA32" s="2"/>
+      <c r="AB32" s="2"/>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>71</v>
       </c>
@@ -3304,57 +3353,58 @@
       <c r="J33" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K33" s="1">
+      <c r="K33" s="2"/>
+      <c r="L33" s="1">
         <v>1334.9594999999999</v>
       </c>
-      <c r="L33" s="1">
+      <c r="M33" s="1">
         <v>1332.4085</v>
       </c>
-      <c r="M33" s="1">
+      <c r="N33" s="1">
         <v>140.36749</v>
       </c>
-      <c r="N33" s="1">
+      <c r="O33" s="1">
         <v>140.22863000000001</v>
       </c>
-      <c r="O33" s="1">
+      <c r="P33" s="1">
         <v>890.56676000000004</v>
       </c>
-      <c r="P33" s="1">
+      <c r="Q33" s="1">
         <v>867.52495999999996</v>
       </c>
-      <c r="Q33" s="1">
+      <c r="R33" s="1">
         <v>181.97694000000001</v>
       </c>
-      <c r="R33" s="1">
+      <c r="S33" s="1">
         <v>167.58100999999999</v>
       </c>
-      <c r="S33" s="1">
+      <c r="T33" s="1">
         <v>326.04685519999998</v>
       </c>
-      <c r="T33" s="1">
+      <c r="U33" s="1">
         <v>329.90475650000002</v>
       </c>
-      <c r="U33" s="1">
+      <c r="V33" s="1">
         <v>420.55824940000002</v>
       </c>
-      <c r="V33" s="1">
+      <c r="W33" s="1">
         <v>416.20577789999999</v>
       </c>
-      <c r="W33" s="1">
+      <c r="X33" s="1">
         <v>6.1403768599999999</v>
       </c>
-      <c r="X33" s="1">
+      <c r="Y33" s="1">
         <v>6.2960675669999997</v>
       </c>
-      <c r="Y33" s="1">
+      <c r="Z33" s="1">
         <v>1045.7004629999999</v>
       </c>
-      <c r="Z33" s="1">
+      <c r="AA33" s="1">
         <v>1039.3456329999999</v>
       </c>
-      <c r="AA33" s="2"/>
+      <c r="AB33" s="2"/>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>75</v>
       </c>
@@ -3381,57 +3431,58 @@
       <c r="J34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K34" s="1">
+      <c r="K34" s="2"/>
+      <c r="L34" s="1">
         <v>710.42561000000001</v>
       </c>
-      <c r="L34" s="1">
+      <c r="M34" s="1">
         <v>722.10673999999995</v>
       </c>
-      <c r="M34" s="1">
+      <c r="N34" s="1">
         <v>259.45987000000002</v>
       </c>
-      <c r="N34" s="1">
+      <c r="O34" s="1">
         <v>255.74288000000001</v>
       </c>
-      <c r="O34" s="1">
+      <c r="P34" s="1">
         <v>617.96151999999995</v>
       </c>
-      <c r="P34" s="1">
+      <c r="Q34" s="1">
         <v>667.95833000000005</v>
       </c>
-      <c r="Q34" s="1">
+      <c r="R34" s="1">
         <v>192.94571999999999</v>
       </c>
-      <c r="R34" s="1">
+      <c r="S34" s="1">
         <v>216.61378999999999</v>
       </c>
-      <c r="S34" s="1">
+      <c r="T34" s="1">
         <v>220.71233000000001</v>
       </c>
-      <c r="T34" s="1">
+      <c r="U34" s="1">
         <v>215.00614999999999</v>
       </c>
-      <c r="U34" s="1">
+      <c r="V34" s="1">
         <v>296.38125000000002</v>
       </c>
-      <c r="V34" s="1">
+      <c r="W34" s="1">
         <v>285.73442</v>
       </c>
-      <c r="W34" s="1">
+      <c r="X34" s="1">
         <v>4.8480699999999999</v>
       </c>
-      <c r="X34" s="1">
+      <c r="Y34" s="1">
         <v>4.8082500000000001</v>
       </c>
-      <c r="Y34" s="1">
+      <c r="Z34" s="1">
         <v>974.42361000000005</v>
       </c>
-      <c r="Z34" s="1">
+      <c r="AA34" s="1">
         <v>975.74207999999999</v>
       </c>
-      <c r="AA34" s="2"/>
+      <c r="AB34" s="2"/>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
@@ -3458,57 +3509,58 @@
       <c r="J35" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K35" s="1">
+      <c r="K35" s="2"/>
+      <c r="L35" s="1">
         <v>987.97864000000004</v>
       </c>
-      <c r="L35" s="1">
+      <c r="M35" s="1">
         <v>1023.88431</v>
       </c>
-      <c r="M35" s="1">
+      <c r="N35" s="1">
         <v>136.90940000000001</v>
       </c>
-      <c r="N35" s="1">
+      <c r="O35" s="1">
         <v>125.55022</v>
       </c>
-      <c r="O35" s="1">
+      <c r="P35" s="1">
         <v>848.00387000000001</v>
       </c>
-      <c r="P35" s="1">
+      <c r="Q35" s="1">
         <v>911.59501</v>
       </c>
-      <c r="Q35" s="1">
+      <c r="R35" s="1">
         <v>146.03609</v>
       </c>
-      <c r="R35" s="1">
+      <c r="S35" s="1">
         <v>152.39292</v>
       </c>
-      <c r="S35" s="1">
+      <c r="T35" s="1">
         <v>270.96600136491787</v>
       </c>
-      <c r="T35" s="1">
+      <c r="U35" s="1">
         <v>293.61016065737721</v>
       </c>
-      <c r="U35" s="1">
+      <c r="V35" s="1">
         <v>328.98322269197018</v>
       </c>
-      <c r="V35" s="1">
+      <c r="W35" s="1">
         <v>358.27343530351908</v>
       </c>
-      <c r="W35" s="1">
+      <c r="X35" s="1">
         <v>5.9904168599777501</v>
       </c>
-      <c r="X35" s="1">
+      <c r="Y35" s="1">
         <v>6.1657277201974576</v>
       </c>
-      <c r="Y35" s="1">
+      <c r="Z35" s="1">
         <v>1043.2016808321439</v>
       </c>
-      <c r="Z35" s="1">
+      <c r="AA35" s="1">
         <v>1033.8370666073399</v>
       </c>
-      <c r="AA35" s="2"/>
+      <c r="AB35" s="2"/>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>64</v>
       </c>
@@ -3535,57 +3587,58 @@
       <c r="J36" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K36" s="1">
+      <c r="K36" s="2"/>
+      <c r="L36" s="1">
         <v>588.15566000000001</v>
       </c>
-      <c r="L36" s="1">
+      <c r="M36" s="1">
         <v>581.03498000000002</v>
       </c>
-      <c r="M36" s="1">
+      <c r="N36" s="1">
         <v>144.82007999999999</v>
       </c>
-      <c r="N36" s="1">
+      <c r="O36" s="1">
         <v>142.07908</v>
       </c>
-      <c r="O36" s="1">
+      <c r="P36" s="1">
         <v>434.04432000000003</v>
       </c>
-      <c r="P36" s="1">
+      <c r="Q36" s="1">
         <v>467.95477</v>
       </c>
-      <c r="Q36" s="1">
+      <c r="R36" s="1">
         <v>164.28407000000001</v>
       </c>
-      <c r="R36" s="1">
+      <c r="S36" s="1">
         <v>174.50191000000001</v>
       </c>
-      <c r="S36" s="1">
+      <c r="T36" s="1">
         <v>165.92209396907029</v>
       </c>
-      <c r="T36" s="1">
+      <c r="U36" s="1">
         <v>174.9936262624575</v>
       </c>
-      <c r="U36" s="1">
+      <c r="V36" s="1">
         <v>211.5404382432672</v>
       </c>
-      <c r="V36" s="1">
+      <c r="W36" s="1">
         <v>217.65706968053911</v>
       </c>
-      <c r="W36" s="1">
+      <c r="X36" s="1">
         <v>4.3983782826139981</v>
       </c>
-      <c r="X36" s="1">
+      <c r="Y36" s="1">
         <v>4.6290699796628756</v>
       </c>
-      <c r="Y36" s="1">
+      <c r="Z36" s="1">
         <v>979.55839685485432</v>
       </c>
-      <c r="Z36" s="1">
+      <c r="AA36" s="1">
         <v>968.92363630364389</v>
       </c>
-      <c r="AA36" s="2"/>
+      <c r="AB36" s="2"/>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>60</v>
       </c>
@@ -3612,57 +3665,58 @@
       <c r="J37" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K37" s="1">
+      <c r="K37" s="2"/>
+      <c r="L37" s="1">
         <v>796.95277999999996</v>
       </c>
-      <c r="L37" s="1">
+      <c r="M37" s="1">
         <v>803.94708000000003</v>
       </c>
-      <c r="M37" s="1">
+      <c r="N37" s="1">
         <v>196.78665000000001</v>
       </c>
-      <c r="N37" s="1">
+      <c r="O37" s="1">
         <v>193.41468</v>
       </c>
-      <c r="O37" s="1">
+      <c r="P37" s="1">
         <v>467.13956999999999</v>
       </c>
-      <c r="P37" s="1">
+      <c r="Q37" s="1">
         <v>469.63520999999997</v>
       </c>
-      <c r="Q37" s="1">
+      <c r="R37" s="1">
         <v>141.06551999999999</v>
       </c>
-      <c r="R37" s="1">
+      <c r="S37" s="1">
         <v>148.61617000000001</v>
       </c>
-      <c r="S37" s="1">
+      <c r="T37" s="1">
         <v>171.54776000000001</v>
       </c>
-      <c r="T37" s="1">
+      <c r="U37" s="1">
         <v>174.12365</v>
       </c>
-      <c r="U37" s="1">
+      <c r="V37" s="1">
         <v>235.67335</v>
       </c>
-      <c r="V37" s="1">
+      <c r="W37" s="1">
         <v>234.00145000000001</v>
       </c>
-      <c r="W37" s="1">
+      <c r="X37" s="1">
         <v>4.0991999999999997</v>
       </c>
-      <c r="X37" s="1">
+      <c r="Y37" s="1">
         <v>4.2719199999999997</v>
       </c>
-      <c r="Y37" s="1">
+      <c r="Z37" s="1">
         <v>952.85733000000005</v>
       </c>
-      <c r="Z37" s="1">
+      <c r="AA37" s="1">
         <v>949.02860999999996</v>
       </c>
-      <c r="AA37" s="2"/>
+      <c r="AB37" s="2"/>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>74</v>
       </c>
@@ -3689,57 +3743,58 @@
       <c r="J38" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K38" s="1">
+      <c r="K38" s="2"/>
+      <c r="L38" s="1">
         <v>745.84932000000003</v>
       </c>
-      <c r="L38" s="1">
+      <c r="M38" s="1">
         <v>724.78371000000004</v>
       </c>
-      <c r="M38" s="1">
+      <c r="N38" s="1">
         <v>174.67984000000001</v>
       </c>
-      <c r="N38" s="1">
+      <c r="O38" s="1">
         <v>184.10452000000001</v>
       </c>
-      <c r="O38" s="1">
+      <c r="P38" s="1">
         <v>640.89274999999998</v>
       </c>
-      <c r="P38" s="1">
+      <c r="Q38" s="1">
         <v>713.59555999999998</v>
       </c>
-      <c r="Q38" s="1">
+      <c r="R38" s="1">
         <v>207.43244999999999</v>
       </c>
-      <c r="R38" s="1">
+      <c r="S38" s="1">
         <v>217.13254000000001</v>
       </c>
-      <c r="S38" s="1">
+      <c r="T38" s="1">
         <v>202.09133</v>
       </c>
-      <c r="T38" s="1">
+      <c r="U38" s="1">
         <v>190.92044999999999</v>
       </c>
-      <c r="U38" s="1">
+      <c r="V38" s="1">
         <v>268.09976999999998</v>
       </c>
-      <c r="V38" s="1">
+      <c r="W38" s="1">
         <v>252.03883999999999</v>
       </c>
-      <c r="W38" s="1">
+      <c r="X38" s="1">
         <v>4.6396199999999999</v>
       </c>
-      <c r="X38" s="1">
+      <c r="Y38" s="1">
         <v>4.4900099999999998</v>
       </c>
-      <c r="Y38" s="1">
+      <c r="Z38" s="1">
         <v>983.9076</v>
       </c>
-      <c r="Z38" s="1">
+      <c r="AA38" s="1">
         <v>979.10626000000002</v>
       </c>
-      <c r="AA38" s="2"/>
+      <c r="AB38" s="2"/>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>73</v>
       </c>
@@ -3766,57 +3821,58 @@
       <c r="J39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K39" s="1">
+      <c r="K39" s="2"/>
+      <c r="L39" s="1">
         <v>1026.50289</v>
       </c>
-      <c r="L39" s="1">
+      <c r="M39" s="1">
         <v>1020.9917799999999</v>
       </c>
-      <c r="M39" s="1">
+      <c r="N39" s="1">
         <v>162.89028999999999</v>
       </c>
-      <c r="N39" s="1">
+      <c r="O39" s="1">
         <v>141.84808000000001</v>
       </c>
-      <c r="O39" s="1">
+      <c r="P39" s="1">
         <v>697.56998999999996</v>
       </c>
-      <c r="P39" s="1">
+      <c r="Q39" s="1">
         <v>756.70920999999998</v>
       </c>
-      <c r="Q39" s="1">
+      <c r="R39" s="1">
         <v>197.1103</v>
       </c>
-      <c r="R39" s="1">
+      <c r="S39" s="1">
         <v>190.01580999999999</v>
       </c>
-      <c r="S39" s="1">
+      <c r="T39" s="1">
         <v>289.11864000000003</v>
       </c>
-      <c r="T39" s="1">
+      <c r="U39" s="1">
         <v>291.79216000000002</v>
       </c>
-      <c r="U39" s="1">
+      <c r="V39" s="1">
         <v>381.45046000000002</v>
       </c>
-      <c r="V39" s="1">
+      <c r="W39" s="1">
         <v>382.83616000000001</v>
       </c>
-      <c r="W39" s="1">
+      <c r="X39" s="1">
         <v>5.5982700000000003</v>
       </c>
-      <c r="X39" s="1">
+      <c r="Y39" s="1">
         <v>5.6699900000000003</v>
       </c>
-      <c r="Y39" s="1">
+      <c r="Z39" s="1">
         <v>1031.7125599999999</v>
       </c>
-      <c r="Z39" s="1">
+      <c r="AA39" s="1">
         <v>1029.29683</v>
       </c>
-      <c r="AA39" s="2"/>
+      <c r="AB39" s="2"/>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>65</v>
       </c>
@@ -3843,57 +3899,58 @@
       <c r="J40" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K40" s="1">
+      <c r="K40" s="2"/>
+      <c r="L40" s="1">
         <v>755.97168999999997</v>
       </c>
-      <c r="L40" s="1">
+      <c r="M40" s="1">
         <v>749.46738000000005</v>
       </c>
-      <c r="M40" s="1">
+      <c r="N40" s="1">
         <v>126.75212000000001</v>
       </c>
-      <c r="N40" s="1">
+      <c r="O40" s="1">
         <v>127.59917</v>
       </c>
-      <c r="O40" s="1">
+      <c r="P40" s="1">
         <v>508.64895000000001</v>
       </c>
-      <c r="P40" s="1">
+      <c r="Q40" s="1">
         <v>491.03690999999998</v>
       </c>
-      <c r="Q40" s="1">
+      <c r="R40" s="1">
         <v>114.96849</v>
       </c>
-      <c r="R40" s="1">
+      <c r="S40" s="1">
         <v>124.59694</v>
       </c>
-      <c r="S40" s="1">
+      <c r="T40" s="1">
         <v>218.18856455650521</v>
       </c>
-      <c r="T40" s="1">
+      <c r="U40" s="1">
         <v>213.81588053186451</v>
       </c>
-      <c r="U40" s="1">
+      <c r="V40" s="1">
         <v>262.97812339734338</v>
       </c>
-      <c r="V40" s="1">
+      <c r="W40" s="1">
         <v>265.11102090427431</v>
       </c>
-      <c r="W40" s="1">
+      <c r="X40" s="1">
         <v>5.3694454672508076</v>
       </c>
-      <c r="X40" s="1">
+      <c r="Y40" s="1">
         <v>5.213865580889621</v>
       </c>
-      <c r="Y40" s="1">
+      <c r="Z40" s="1">
         <v>1034.0471637017549</v>
       </c>
-      <c r="Z40" s="1">
+      <c r="AA40" s="1">
         <v>1022.323317866214</v>
       </c>
-      <c r="AA40" s="2"/>
+      <c r="AB40" s="2"/>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>70</v>
       </c>
@@ -3920,59 +3977,60 @@
       <c r="J41" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K41" s="1">
+      <c r="K41" s="2"/>
+      <c r="L41" s="1">
         <v>976.20858999999996</v>
       </c>
-      <c r="L41" s="1">
+      <c r="M41" s="1">
         <v>1018.0701</v>
       </c>
-      <c r="M41" s="1">
+      <c r="N41" s="1">
         <v>106.54422</v>
       </c>
-      <c r="N41" s="1">
+      <c r="O41" s="1">
         <v>114.72417</v>
       </c>
-      <c r="O41" s="1">
+      <c r="P41" s="1">
         <v>820.69983999999999</v>
       </c>
-      <c r="P41" s="1">
+      <c r="Q41" s="1">
         <v>811.04602999999997</v>
       </c>
-      <c r="Q41" s="1">
+      <c r="R41" s="1">
         <v>140.59798000000001</v>
       </c>
-      <c r="R41" s="1">
+      <c r="S41" s="1">
         <v>137.31433999999999</v>
       </c>
-      <c r="S41" s="1">
+      <c r="T41" s="1">
         <v>193.81800000000001</v>
       </c>
-      <c r="T41" s="1">
+      <c r="U41" s="1">
         <v>200.7965098</v>
       </c>
-      <c r="U41" s="1">
+      <c r="V41" s="1">
         <v>265.63274999999999</v>
       </c>
-      <c r="V41" s="1">
+      <c r="W41" s="1">
         <v>270.35505890000002</v>
       </c>
-      <c r="W41" s="1">
+      <c r="X41" s="1">
         <v>4.4177099999999996</v>
       </c>
-      <c r="X41" s="1">
+      <c r="Y41" s="1">
         <v>4.5538077079999999</v>
       </c>
-      <c r="Y41" s="1">
+      <c r="Z41" s="1">
         <v>1012.94936</v>
       </c>
-      <c r="Z41" s="1">
+      <c r="AA41" s="1">
         <v>1010.1170100000001</v>
       </c>
-      <c r="AA41" s="2"/>
+      <c r="AB41" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="K1:Z1"/>
+    <mergeCell ref="L1:AA1"/>
     <mergeCell ref="B1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>